<commit_message>
Resistors R4 and R2 updated for measuring 1S battery
</commit_message>
<xml_diff>
--- a/Cálculos-14500.xlsx
+++ b/Cálculos-14500.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ihr/ZigbeeGasMeter/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC24647A-07C7-2940-B87E-F0035E2F8F74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FA36E2F-B244-2B43-874F-C3EE58BB4066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="200" yWindow="620" windowWidth="41660" windowHeight="13680" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -206,18 +206,12 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -260,13 +254,13 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1031,8 +1025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C2:W1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P55" sqref="P55"/>
+    <sheetView tabSelected="1" topLeftCell="E66" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O47" sqref="O47:P47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1767,10 +1761,10 @@
       </c>
     </row>
     <row r="47" spans="12:23" ht="16" x14ac:dyDescent="0.2">
-      <c r="O47" s="9">
+      <c r="O47" s="14">
         <v>570000</v>
       </c>
-      <c r="P47" s="10">
+      <c r="P47" s="15">
         <f t="shared" si="4"/>
         <v>2089999.9999999991</v>
       </c>
@@ -1930,7 +1924,7 @@
       <c r="S57" t="s">
         <v>39</v>
       </c>
-      <c r="T57" s="11">
+      <c r="T57" s="9">
         <f>R57/P57</f>
         <v>1.2699999999999998</v>
       </c>
@@ -2020,7 +2014,7 @@
       </c>
     </row>
     <row r="66" spans="15:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="P66" s="12"/>
+      <c r="P66" s="10"/>
       <c r="R66">
         <f>P65/R64</f>
         <v>3.6666666666666652</v>
@@ -2048,7 +2042,7 @@
         <v>100000</v>
       </c>
       <c r="P69" s="7">
-        <f t="shared" ref="P69:P85" si="8">O69*R$66</f>
+        <f t="shared" ref="P69:P84" si="8">O69*R$66</f>
         <v>366666.66666666651</v>
       </c>
       <c r="Q69" s="8">
@@ -2393,10 +2387,10 @@
       <c r="M85" t="s">
         <v>46</v>
       </c>
-      <c r="O85" s="14">
+      <c r="O85" s="12">
         <v>100000</v>
       </c>
-      <c r="P85" s="15">
+      <c r="P85" s="13">
         <v>390000</v>
       </c>
       <c r="Q85" s="8">
@@ -2414,7 +2408,7 @@
       <c r="U85">
         <v>4.2</v>
       </c>
-      <c r="V85" s="13">
+      <c r="V85" s="11">
         <f>U85/S85</f>
         <v>3.342857142857143</v>
       </c>

</xml_diff>